<commit_message>
update publications and patents
</commit_message>
<xml_diff>
--- a/markdown_generator/patents.xlsx
+++ b/markdown_generator/patents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\yanhu\markdown_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2B75AE-ED25-430D-AA6A-4BE4043A9700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A37591-2127-4DC4-A33D-301FCF808BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6300" yWindow="3270" windowWidth="26630" windowHeight="17000" xr2:uid="{76ADD6EB-04CE-4B45-9814-C5A179BE9D48}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>2022112938120</t>
   </si>
   <si>
-    <t>金日初，刘江，胡衍，缪函霈，姜泓羊，王星月，曾娜，叶海礼</t>
-  </si>
-  <si>
     <t>胡衍, 邱忠喜, 张嘉奇, 孙沛铖, 刘江</t>
   </si>
   <si>
@@ -200,6 +197,10 @@
   </si>
   <si>
     <t>刘江,东田理沙,张颖麟,章晓庆,刘鹏,杨冰,胡衍,李衡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金日初,刘江,胡衍,缪函霈,姜泓羊,王星月,曾娜,叶海礼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -616,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7972B91-56B3-4775-99B7-4CEA9511C314}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="A1:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -628,79 +629,79 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="8" t="s">
         <v>1</v>
       </c>
@@ -708,15 +709,15 @@
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -725,15 +726,15 @@
         <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -742,15 +743,15 @@
         <v>2</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -759,15 +760,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
@@ -776,15 +777,15 @@
         <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
@@ -793,15 +794,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -810,15 +811,15 @@
         <v>2</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -827,15 +828,15 @@
         <v>2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1</v>
@@ -844,15 +845,15 @@
         <v>2</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
@@ -861,15 +862,15 @@
         <v>2</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
@@ -878,15 +879,15 @@
         <v>2</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
@@ -895,12 +896,12 @@
         <v>2</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
update patents and publications
</commit_message>
<xml_diff>
--- a/markdown_generator/patents.xlsx
+++ b/markdown_generator/patents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\yanhu\markdown_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A37591-2127-4DC4-A33D-301FCF808BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59119AE4-AFC7-467E-84CB-526106946D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="3270" windowWidth="26630" windowHeight="17000" xr2:uid="{76ADD6EB-04CE-4B45-9814-C5A179BE9D48}"/>
+    <workbookView xWindow="15240" yWindow="830" windowWidth="26580" windowHeight="17020" xr2:uid="{76ADD6EB-04CE-4B45-9814-C5A179BE9D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>基于特征一致性的眼底图像增强方法、系统、设备及介质</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -201,6 +201,48 @@
   </si>
   <si>
     <t>金日初,刘江,胡衍,缪函霈,姜泓羊,王星月,曾娜,叶海礼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘江,胡衍,叶海礼,陈晓慧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>眼底图像预测方法、眼底图像预测系统、设备及存储介质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023102311682</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘江,胡衍,沈俊勇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>病变检测模型的训练方法和装置、电子设备及存储介质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023105094659</t>
+  </si>
+  <si>
+    <t>受理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘江,李衡,俞向阳,区明阳,李昊锦,胡衍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>医学图像生成方法、装置、电子设备及存储介质</t>
+  </si>
+  <si>
+    <t>发明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023108192704</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -270,7 +312,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -300,6 +342,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7972B91-56B3-4775-99B7-4CEA9511C314}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -910,18 +955,62 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+    <row r="18" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E17" xr:uid="{E7972B91-56B3-4775-99B7-4CEA9511C314}"/>

</xml_diff>